<commit_message>
changed test cases list
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>Column</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>include in vcf testing?</t>
+  </si>
+  <si>
+    <t>what is this? never shows a value in any of my inputs</t>
+  </si>
+  <si>
+    <t>needed? very simple test</t>
   </si>
 </sst>
 </file>
@@ -621,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1310,6 +1316,9 @@
       <c r="B57" t="s">
         <v>64</v>
       </c>
+      <c r="E57" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -1317,6 +1326,15 @@
       </c>
       <c r="B58" t="s">
         <v>65</v>
+      </c>
+      <c r="C58" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated exac to include esp6500 data
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
   <si>
     <t>Column</t>
   </si>
@@ -273,7 +273,13 @@
     <t>what is this? never shows a value in any of my inputs</t>
   </si>
   <si>
-    <t>needed? very simple test</t>
+    <t xml:space="preserve">very simple. unclear how CRAVAT decides when to make a mupit link.  </t>
+  </si>
+  <si>
+    <t>when does CRAVAT decide to make a pubmed link? some vars in 1000v run have no pubmed hits, but tried to make pubmed link anyway</t>
+  </si>
+  <si>
+    <t>when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in exac input</t>
   </si>
 </sst>
 </file>
@@ -627,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -955,76 +961,121 @@
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9</v>
+      </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9</v>
+      </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
       <c r="B25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
       <c r="B26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
       <c r="B28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
       <c r="B29" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
       <c r="B30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9</v>
+      </c>
       <c r="B31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9</v>
+      </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
       <c r="B33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9</v>
+      </c>
       <c r="B34" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
       <c r="B35" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9</v>
+      </c>
       <c r="B36" t="s">
         <v>33</v>
       </c>
@@ -1157,6 +1208,15 @@
       <c r="B45" t="s">
         <v>42</v>
       </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -1177,13 +1237,25 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10</v>
+      </c>
       <c r="B48" t="s">
         <v>55</v>
       </c>
@@ -1197,7 +1269,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>10</v>
+      </c>
       <c r="B49" t="s">
         <v>61</v>
       </c>
@@ -1211,7 +1286,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
       <c r="B50" t="s">
         <v>56</v>
       </c>
@@ -1225,7 +1303,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10</v>
+      </c>
       <c r="B51" t="s">
         <v>57</v>
       </c>
@@ -1239,7 +1320,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>10</v>
+      </c>
       <c r="B52" t="s">
         <v>58</v>
       </c>
@@ -1253,7 +1337,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
       <c r="B53" t="s">
         <v>59</v>
       </c>
@@ -1267,7 +1354,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10</v>
+      </c>
       <c r="B54" t="s">
         <v>60</v>
       </c>
@@ -1281,7 +1371,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10</v>
+      </c>
       <c r="B55" t="s">
         <v>62</v>
       </c>
@@ -1295,7 +1388,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10</v>
+      </c>
       <c r="B56" t="s">
         <v>63</v>
       </c>
@@ -1309,12 +1405,18 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
       <c r="B57" t="s">
         <v>64</v>
+      </c>
+      <c r="C57" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" t="s">
+        <v>79</v>
       </c>
       <c r="E57" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
renamed exac to pop_stats
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -231,9 +231,6 @@
     <t>could be bug, mix up btwn variant reads, sample reads</t>
   </si>
   <si>
-    <t>exac</t>
-  </si>
-  <si>
     <t>failing hard</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in exac input</t>
+  </si>
+  <si>
+    <t>pop_stats</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -670,10 +670,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,10 +698,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,10 +726,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,10 +824,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
         <v>69</v>
@@ -875,10 +875,10 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
         <v>75</v>
-      </c>
-      <c r="E16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -934,13 +934,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,13 +951,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1091,7 +1091,7 @@
         <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1105,10 +1105,10 @@
         <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,10 +1147,10 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,13 +1192,13 @@
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1209,13 +1209,13 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,13 +1226,13 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,10 +1246,10 @@
         <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1263,10 +1263,10 @@
         <v>21</v>
       </c>
       <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" t="s">
         <v>70</v>
-      </c>
-      <c r="E48" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1280,10 +1280,10 @@
         <v>21</v>
       </c>
       <c r="D49" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" t="s">
         <v>70</v>
-      </c>
-      <c r="E49" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1297,10 +1297,10 @@
         <v>21</v>
       </c>
       <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" t="s">
         <v>70</v>
-      </c>
-      <c r="E50" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1314,10 +1314,10 @@
         <v>21</v>
       </c>
       <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" t="s">
         <v>70</v>
-      </c>
-      <c r="E51" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1331,10 +1331,10 @@
         <v>21</v>
       </c>
       <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
         <v>70</v>
-      </c>
-      <c r="E52" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1348,10 +1348,10 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" t="s">
         <v>70</v>
-      </c>
-      <c r="E53" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1365,10 +1365,10 @@
         <v>21</v>
       </c>
       <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" t="s">
         <v>70</v>
-      </c>
-      <c r="E54" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1382,10 +1382,10 @@
         <v>21</v>
       </c>
       <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" t="s">
         <v>70</v>
-      </c>
-      <c r="E55" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1399,10 +1399,10 @@
         <v>21</v>
       </c>
       <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" t="s">
         <v>70</v>
-      </c>
-      <c r="E56" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1413,13 +1413,13 @@
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,13 +1430,13 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,13 +1447,13 @@
         <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test cases list
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -270,16 +270,16 @@
     <t>what is this? never shows a value in any of my inputs</t>
   </si>
   <si>
-    <t xml:space="preserve">very simple. unclear how CRAVAT decides when to make a mupit link.  </t>
-  </si>
-  <si>
     <t>when does CRAVAT decide to make a pubmed link? some vars in 1000v run have no pubmed hits, but tried to make pubmed link anyway</t>
   </si>
   <si>
-    <t>when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in exac input</t>
-  </si>
-  <si>
     <t>pop_stats</t>
+  </si>
+  <si>
+    <t>out of date. also, when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in pop_stats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">should be simple. unclear how CRAVAT decides when to make a mupit link.  </t>
   </si>
 </sst>
 </file>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -928,7 +928,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1215,7 +1215,7 @@
         <v>78</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
         <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E47" t="s">
         <v>85</v>
@@ -1263,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
         <v>70</v>
@@ -1280,7 +1280,7 @@
         <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E49" t="s">
         <v>70</v>
@@ -1297,7 +1297,7 @@
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E50" t="s">
         <v>70</v>
@@ -1314,7 +1314,7 @@
         <v>21</v>
       </c>
       <c r="D51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E51" t="s">
         <v>70</v>
@@ -1331,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E52" t="s">
         <v>70</v>
@@ -1348,7 +1348,7 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E53" t="s">
         <v>70</v>
@@ -1365,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="D54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E54" t="s">
         <v>70</v>
@@ -1382,7 +1382,7 @@
         <v>21</v>
       </c>
       <c r="D55" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E55" t="s">
         <v>70</v>
@@ -1399,7 +1399,7 @@
         <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E56" t="s">
         <v>70</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
         <v>64</v>
@@ -1419,7 +1419,7 @@
         <v>78</v>
       </c>
       <c r="E57" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1441,7 +1441,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
updated Test List, added rouding test case
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -249,37 +249,37 @@
     <t>one wrong result</t>
   </si>
   <si>
-    <t>unclear how CRAVAT looks these up</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
-    <t>will update too frequently to make effective test</t>
-  </si>
-  <si>
-    <t>can't find where number CRAVAT reports is on 1000G website</t>
-  </si>
-  <si>
     <t>include in vcf testing?</t>
   </si>
   <si>
-    <t>what is this? never shows a value in any of my inputs</t>
-  </si>
-  <si>
-    <t>when does CRAVAT decide to make a pubmed link? some vars in 1000v run have no pubmed hits, but tried to make pubmed link anyway</t>
-  </si>
-  <si>
     <t>pop_stats</t>
   </si>
   <si>
     <t>out of date. also, when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in pop_stats</t>
   </si>
   <si>
-    <t xml:space="preserve">should be simple. unclear how CRAVAT decides when to make a mupit link.  </t>
-  </si>
-  <si>
     <t>CRAVAT db not matching any available dbs. xls files in testing folder</t>
+  </si>
+  <si>
+    <t>browser.1000genomes.com</t>
+  </si>
+  <si>
+    <t>regtest for now, use mupit to find aas in hotspots on certain genes</t>
+  </si>
+  <si>
+    <t>regtest for now, use genes available in mupit</t>
+  </si>
+  <si>
+    <t>test just for a ballpark figure</t>
+  </si>
+  <si>
+    <t>all vars with pubmed hits should have a pubmed link</t>
+  </si>
+  <si>
+    <t>retest, look up in refsew, ensembl</t>
   </si>
 </sst>
 </file>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -824,10 +824,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
         <v>69</v>
@@ -934,13 +934,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,13 +951,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>72</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1209,13 +1209,13 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,13 +1226,13 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,10 +1246,10 @@
         <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1263,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E48" t="s">
         <v>70</v>
@@ -1280,7 +1280,7 @@
         <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E49" t="s">
         <v>70</v>
@@ -1297,7 +1297,7 @@
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E50" t="s">
         <v>70</v>
@@ -1314,7 +1314,7 @@
         <v>21</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E51" t="s">
         <v>70</v>
@@ -1331,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E52" t="s">
         <v>70</v>
@@ -1348,7 +1348,7 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E53" t="s">
         <v>70</v>
@@ -1365,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="D54" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E54" t="s">
         <v>70</v>
@@ -1382,7 +1382,7 @@
         <v>21</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E55" t="s">
         <v>70</v>
@@ -1399,7 +1399,7 @@
         <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E56" t="s">
         <v>70</v>
@@ -1413,13 +1413,13 @@
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,13 +1430,13 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E58" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,13 +1447,13 @@
         <v>66</v>
       </c>
       <c r="C59" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" t="s">
         <v>77</v>
-      </c>
-      <c r="D59" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transcript test case, added string_included verification method
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="88">
   <si>
     <t>Column</t>
   </si>
@@ -279,7 +279,10 @@
     <t>all vars with pubmed hits should have a pubmed link</t>
   </si>
   <si>
-    <t>retest, look up in refsew, ensembl</t>
+    <t>just regtest</t>
+  </si>
+  <si>
+    <t>transcript</t>
   </si>
 </sst>
 </file>
@@ -633,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -928,16 +931,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s">
         <v>86</v>
@@ -945,16 +948,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
made pubmed test. wont work yet, need to add more options to submission parameters
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
   <si>
     <t>Column</t>
   </si>
@@ -273,16 +273,13 @@
     <t>regtest for now, use genes available in mupit</t>
   </si>
   <si>
-    <t>test just for a ballpark figure</t>
-  </si>
-  <si>
-    <t>all vars with pubmed hits should have a pubmed link</t>
-  </si>
-  <si>
     <t>just regtest</t>
   </si>
   <si>
     <t>transcript</t>
+  </si>
+  <si>
+    <t>HOW TO INCLUDE PUBMED USING REQUESTS MODULE</t>
   </si>
 </sst>
 </file>
@@ -637,7 +634,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -940,10 +937,10 @@
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,10 +954,10 @@
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1195,13 +1192,13 @@
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,7 +1215,7 @@
         <v>76</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added kg to pop_stats
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
   <si>
     <t>Column</t>
   </si>
@@ -105,9 +105,6 @@
     <t>protein_change</t>
   </si>
   <si>
-    <t>needs upgrading</t>
-  </si>
-  <si>
     <t>chasm p value</t>
   </si>
   <si>
@@ -261,12 +258,6 @@
     <t>out of date. also, when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in pop_stats</t>
   </si>
   <si>
-    <t>CRAVAT db not matching any available dbs. xls files in testing folder</t>
-  </si>
-  <si>
-    <t>browser.1000genomes.com</t>
-  </si>
-  <si>
     <t>regtest for now, use mupit to find aas in hotspots on certain genes</t>
   </si>
   <si>
@@ -279,7 +270,13 @@
     <t>transcript</t>
   </si>
   <si>
-    <t>HOW TO INCLUDE PUBMED USING REQUESTS MODULE</t>
+    <t>pubmed</t>
+  </si>
+  <si>
+    <t>CRAVAT db not matching any available dbs.     xls files in testing folder</t>
+  </si>
+  <si>
+    <t>failures in NC regions</t>
   </si>
 </sst>
 </file>
@@ -633,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -647,7 +644,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -670,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,10 +695,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,10 +723,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,13 +821,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -847,7 +844,7 @@
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -875,10 +872,10 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,9 +919,6 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -937,10 +931,10 @@
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -954,10 +948,10 @@
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -965,7 +959,7 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -973,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -981,7 +975,7 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -989,7 +983,7 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -997,7 +991,7 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1005,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1013,7 +1007,7 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1021,7 +1015,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1029,7 +1023,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1037,7 +1031,7 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1045,7 +1039,7 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1053,7 +1047,7 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1061,7 +1055,7 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1069,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1077,7 +1071,7 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
@@ -1085,13 +1079,13 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1099,16 +1093,16 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1116,13 +1110,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,13 +1124,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1144,13 +1138,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1158,13 +1152,13 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
         <v>21</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,16 +1166,16 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
         <v>21</v>
       </c>
       <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
         <v>67</v>
-      </c>
-      <c r="E43" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1189,50 +1183,50 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E44" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1240,16 +1234,16 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
       </c>
       <c r="D47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" t="s">
         <v>78</v>
-      </c>
-      <c r="E47" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1257,16 +1251,16 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1274,16 +1268,16 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" t="s">
         <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1291,16 +1285,16 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1308,16 +1302,16 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
         <v>21</v>
       </c>
       <c r="D51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1325,16 +1319,16 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
         <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1342,16 +1336,16 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1359,16 +1353,16 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
         <v>21</v>
       </c>
       <c r="D54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1376,16 +1370,16 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
         <v>21</v>
       </c>
       <c r="D55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1393,16 +1387,16 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
         <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
@@ -1410,33 +1404,33 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E57" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E58" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1444,16 +1438,16 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" t="s">
         <v>76</v>
-      </c>
-      <c r="D59" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merget transcript and so_best, renamed seqont
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="156">
   <si>
     <t>Column</t>
   </si>
@@ -482,13 +482,19 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>when does this show up?</t>
+  </si>
+  <si>
+    <t>seqont</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,13 +526,6 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -574,7 +573,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -587,7 +585,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -909,11 +907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,45 +920,45 @@
     <col min="2" max="2" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="13">
         <v>18</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>152</v>
       </c>
     </row>
@@ -974,17 +972,17 @@
       <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="8">
-        <v>1</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -996,17 +994,17 @@
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -1018,17 +1016,17 @@
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -1040,17 +1038,17 @@
       <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1062,17 +1060,17 @@
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1084,22 +1082,22 @@
       <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1113,22 +1111,22 @@
       <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="8">
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1142,22 +1140,22 @@
       <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8">
-        <v>1</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1177,13 +1175,13 @@
       <c r="G10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" s="8">
-        <v>1</v>
-      </c>
-      <c r="J10" s="8">
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1203,13 +1201,13 @@
       <c r="G11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="8">
-        <v>1</v>
-      </c>
-      <c r="I11" s="8">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1226,22 +1224,22 @@
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="8">
-        <v>1</v>
-      </c>
-      <c r="I12" s="8">
-        <v>1</v>
-      </c>
-      <c r="J12" s="8">
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
         <v>1</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1258,22 +1256,22 @@
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="8">
-        <v>1</v>
-      </c>
-      <c r="I13" s="8">
-        <v>1</v>
-      </c>
-      <c r="J13" s="8">
+      <c r="H13" s="7">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1287,27 +1285,27 @@
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="8">
-        <v>1</v>
-      </c>
-      <c r="J14" s="8">
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
@@ -1317,24 +1315,24 @@
       <c r="D15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="11" t="s">
+      <c r="E15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
       <c r="K15" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
@@ -1344,18 +1342,18 @@
       <c r="D16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
       <c r="K16" s="4" t="s">
         <v>71</v>
       </c>
@@ -1370,22 +1368,22 @@
       <c r="D17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="10">
-        <v>1</v>
-      </c>
-      <c r="I17" s="10">
-        <v>1</v>
-      </c>
-      <c r="J17" s="10">
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1</v>
+      </c>
+      <c r="J17" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1399,22 +1397,22 @@
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="8">
-        <v>1</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="10">
-        <v>1</v>
-      </c>
-      <c r="I18" s="10">
-        <v>1</v>
-      </c>
-      <c r="J18" s="10">
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1</v>
+      </c>
+      <c r="J18" s="9">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1431,22 +1429,22 @@
       <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="8">
-        <v>1</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="10">
-        <v>1</v>
-      </c>
-      <c r="I19" s="10">
-        <v>1</v>
-      </c>
-      <c r="J19" s="10">
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
         <v>1</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1463,22 +1461,22 @@
       <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="8">
-        <v>1</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="10">
-        <v>1</v>
-      </c>
-      <c r="I20" s="10">
-        <v>1</v>
-      </c>
-      <c r="J20" s="10">
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1492,22 +1490,22 @@
       <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="10">
-        <v>1</v>
-      </c>
-      <c r="I21" s="10">
-        <v>1</v>
-      </c>
-      <c r="J21" s="10">
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>1</v>
+      </c>
+      <c r="J21" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1521,22 +1519,22 @@
       <c r="D22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="8">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="10">
-        <v>1</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1</v>
-      </c>
-      <c r="J22" s="10">
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1</v>
+      </c>
+      <c r="J22" s="9">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="s">
@@ -1553,22 +1551,22 @@
       <c r="D23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8">
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="10">
-        <v>1</v>
-      </c>
-      <c r="I23" s="10">
-        <v>1</v>
-      </c>
-      <c r="J23" s="10">
+      <c r="H23" s="9">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9">
         <v>1</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -1585,22 +1583,22 @@
       <c r="D24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="8">
-        <v>1</v>
-      </c>
-      <c r="F24" s="8">
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="10">
-        <v>1</v>
-      </c>
-      <c r="I24" s="10">
-        <v>1</v>
-      </c>
-      <c r="J24" s="10">
+      <c r="H24" s="9">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1</v>
+      </c>
+      <c r="J24" s="9">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -1617,22 +1615,22 @@
       <c r="D25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="8">
-        <v>1</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="10">
-        <v>1</v>
-      </c>
-      <c r="I25" s="10">
-        <v>1</v>
-      </c>
-      <c r="J25" s="10">
+      <c r="H25" s="9">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1</v>
+      </c>
+      <c r="J25" s="9">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -1649,22 +1647,22 @@
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="E26" s="7">
+        <v>1</v>
+      </c>
+      <c r="F26" s="7">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="10">
-        <v>1</v>
-      </c>
-      <c r="I26" s="10">
-        <v>1</v>
-      </c>
-      <c r="J26" s="10">
+      <c r="H26" s="9">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1</v>
+      </c>
+      <c r="J26" s="9">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -1681,22 +1679,22 @@
       <c r="D27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="8">
-        <v>1</v>
-      </c>
-      <c r="F27" s="8">
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="7">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="10">
-        <v>1</v>
-      </c>
-      <c r="I27" s="10">
-        <v>1</v>
-      </c>
-      <c r="J27" s="10">
+      <c r="H27" s="9">
+        <v>1</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -1713,22 +1711,22 @@
       <c r="D28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="8">
-        <v>1</v>
-      </c>
-      <c r="F28" s="8">
+      <c r="E28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="10">
-        <v>1</v>
-      </c>
-      <c r="I28" s="10">
-        <v>1</v>
-      </c>
-      <c r="J28" s="10">
+      <c r="H28" s="9">
+        <v>1</v>
+      </c>
+      <c r="I28" s="9">
+        <v>1</v>
+      </c>
+      <c r="J28" s="9">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="s">
@@ -1745,22 +1743,22 @@
       <c r="D29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="8">
-        <v>1</v>
-      </c>
-      <c r="F29" s="8">
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="10">
-        <v>1</v>
-      </c>
-      <c r="I29" s="10">
-        <v>1</v>
-      </c>
-      <c r="J29" s="10">
+      <c r="H29" s="9">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9">
+        <v>1</v>
+      </c>
+      <c r="J29" s="9">
         <v>1</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -1777,22 +1775,22 @@
       <c r="D30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="8">
-        <v>1</v>
-      </c>
-      <c r="F30" s="8">
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="10">
-        <v>1</v>
-      </c>
-      <c r="I30" s="10">
-        <v>1</v>
-      </c>
-      <c r="J30" s="10">
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9">
+        <v>1</v>
+      </c>
+      <c r="J30" s="9">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -1809,22 +1807,22 @@
       <c r="D31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="8">
-        <v>1</v>
-      </c>
-      <c r="F31" s="8">
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="10">
-        <v>1</v>
-      </c>
-      <c r="I31" s="10">
-        <v>1</v>
-      </c>
-      <c r="J31" s="10">
+      <c r="H31" s="9">
+        <v>1</v>
+      </c>
+      <c r="I31" s="9">
+        <v>1</v>
+      </c>
+      <c r="J31" s="9">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="s">
@@ -1841,22 +1839,22 @@
       <c r="D32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="8">
-        <v>1</v>
-      </c>
-      <c r="F32" s="8">
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="10">
-        <v>1</v>
-      </c>
-      <c r="I32" s="10">
-        <v>1</v>
-      </c>
-      <c r="J32" s="10">
+      <c r="H32" s="9">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9">
+        <v>1</v>
+      </c>
+      <c r="J32" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1870,19 +1868,19 @@
       <c r="D33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="10">
-        <v>1</v>
-      </c>
-      <c r="I33" s="10">
-        <v>1</v>
-      </c>
-      <c r="J33" s="10">
+      <c r="H33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9">
+        <v>1</v>
+      </c>
+      <c r="J33" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1896,19 +1894,19 @@
       <c r="D34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H34" s="10">
-        <v>1</v>
-      </c>
-      <c r="I34" s="10">
-        <v>1</v>
-      </c>
-      <c r="J34" s="10">
+      <c r="H34" s="9">
+        <v>1</v>
+      </c>
+      <c r="I34" s="9">
+        <v>1</v>
+      </c>
+      <c r="J34" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1922,22 +1920,22 @@
       <c r="D35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="8">
-        <v>1</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="10">
-        <v>1</v>
-      </c>
-      <c r="I35" s="10">
-        <v>1</v>
-      </c>
-      <c r="J35" s="10">
+        <v>155</v>
+      </c>
+      <c r="H35" s="9">
+        <v>1</v>
+      </c>
+      <c r="I35" s="9">
+        <v>1</v>
+      </c>
+      <c r="J35" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1946,7 +1944,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>86</v>
@@ -1954,17 +1952,17 @@
       <c r="D36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>148</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="10">
-        <v>1</v>
-      </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="H36" s="9">
+        <v>1</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="2" t="s">
         <v>65</v>
       </c>
@@ -1974,7 +1972,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>86</v>
@@ -1982,17 +1980,17 @@
       <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>148</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H37" s="10">
-        <v>1</v>
-      </c>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="H37" s="9">
+        <v>1</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
       <c r="K37" s="2" t="s">
         <v>64</v>
       </c>
@@ -2001,29 +1999,29 @@
       <c r="A38" s="6">
         <v>37</v>
       </c>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="8">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H38" s="10">
-        <v>1</v>
-      </c>
-      <c r="I38" s="10">
-        <v>1</v>
-      </c>
-      <c r="J38" s="10">
-        <v>1</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>84</v>
+        <v>61</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2034,57 +2032,51 @@
         <v>86</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="8">
+        <v>76</v>
+      </c>
+      <c r="E39" s="7">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" s="10">
-        <v>1</v>
-      </c>
-      <c r="I39" s="10">
-        <v>1</v>
-      </c>
-      <c r="J39" s="10">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="H39" s="9">
+        <v>1</v>
+      </c>
+      <c r="I39" s="9">
+        <v>1</v>
+      </c>
+      <c r="J39" s="9">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
-        <v>4</v>
-      </c>
       <c r="C40" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I40" s="8">
-        <v>1</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>55</v>
+        <v>75</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H40" s="9">
+        <v>1</v>
+      </c>
+      <c r="I40" s="9">
+        <v>1</v>
+      </c>
+      <c r="J40" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2098,28 +2090,28 @@
         <v>86</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="7" t="s">
         <v>61</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H41" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I41" s="8">
-        <v>1</v>
-      </c>
-      <c r="J41" s="8" t="s">
+      <c r="H41" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I41" s="7">
+        <v>1</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>153</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2133,47 +2125,53 @@
         <v>86</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H42" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I42" s="8">
-        <v>1</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>153</v>
+      <c r="H42" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>42</v>
       </c>
+      <c r="B43" s="2">
+        <v>4</v>
+      </c>
       <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="8">
-        <v>1</v>
-      </c>
-      <c r="F43" s="8">
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H43" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I43" s="8">
-        <v>1</v>
-      </c>
-      <c r="J43" s="8" t="s">
+      <c r="H43" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I43" s="7">
+        <v>1</v>
+      </c>
+      <c r="J43" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2185,24 +2183,24 @@
         <v>86</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="8">
-        <v>1</v>
-      </c>
-      <c r="F44" s="8">
+        <v>77</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7">
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H44" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I44" s="8">
-        <v>1</v>
-      </c>
-      <c r="J44" s="8" t="s">
+      <c r="H44" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I44" s="7">
+        <v>1</v>
+      </c>
+      <c r="J44" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2214,24 +2212,24 @@
         <v>86</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="8">
-        <v>1</v>
-      </c>
-      <c r="F45" s="8">
+        <v>3</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H45" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I45" s="8">
-        <v>1</v>
-      </c>
-      <c r="J45" s="8" t="s">
+      <c r="H45" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" s="7">
+        <v>1</v>
+      </c>
+      <c r="J45" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2243,24 +2241,24 @@
         <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="8">
-        <v>1</v>
-      </c>
-      <c r="F46" s="8">
+        <v>78</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H46" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I46" s="8">
-        <v>1</v>
-      </c>
-      <c r="J46" s="8" t="s">
+      <c r="H46" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" s="7">
+        <v>1</v>
+      </c>
+      <c r="J46" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2272,24 +2270,24 @@
         <v>86</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="8">
-        <v>1</v>
-      </c>
-      <c r="F47" s="8">
+        <v>79</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7">
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H47" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I47" s="8">
-        <v>1</v>
-      </c>
-      <c r="J47" s="8" t="s">
+      <c r="H47" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" s="7">
+        <v>1</v>
+      </c>
+      <c r="J47" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2301,24 +2299,24 @@
         <v>86</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="8">
-        <v>1</v>
-      </c>
-      <c r="F48" s="8">
+        <v>9</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7">
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H48" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I48" s="8">
-        <v>1</v>
-      </c>
-      <c r="J48" s="8" t="s">
+      <c r="H48" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I48" s="7">
+        <v>1</v>
+      </c>
+      <c r="J48" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2330,24 +2328,24 @@
         <v>86</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="8">
-        <v>1</v>
-      </c>
-      <c r="F49" s="8">
+        <v>10</v>
+      </c>
+      <c r="E49" s="7">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
         <v>1</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H49" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I49" s="8">
-        <v>1</v>
-      </c>
-      <c r="J49" s="8" t="s">
+      <c r="H49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I49" s="7">
+        <v>1</v>
+      </c>
+      <c r="J49" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2359,24 +2357,24 @@
         <v>86</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="8">
-        <v>1</v>
-      </c>
-      <c r="F50" s="8">
+        <v>11</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7">
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H50" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I50" s="8">
-        <v>1</v>
-      </c>
-      <c r="J50" s="8" t="s">
+      <c r="H50" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I50" s="7">
+        <v>1</v>
+      </c>
+      <c r="J50" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2388,24 +2386,24 @@
         <v>86</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="8">
-        <v>1</v>
-      </c>
-      <c r="F51" s="8">
+        <v>5</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1</v>
+      </c>
+      <c r="F51" s="7">
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H51" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I51" s="8">
-        <v>1</v>
-      </c>
-      <c r="J51" s="8" t="s">
+      <c r="H51" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I51" s="7">
+        <v>1</v>
+      </c>
+      <c r="J51" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2417,19 +2415,26 @@
         <v>86</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="8">
+        <v>13</v>
+      </c>
+      <c r="E52" s="7">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7">
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H52" s="10">
-        <v>1</v>
-      </c>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
+        <v>123</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I52" s="7">
+        <v>1</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
@@ -2439,19 +2444,19 @@
         <v>86</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E53" s="8">
+        <v>30</v>
+      </c>
+      <c r="E53" s="7">
         <v>1</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H53" s="10">
-        <v>1</v>
-      </c>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
+      <c r="H53" s="9">
+        <v>1</v>
+      </c>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
@@ -2461,19 +2466,19 @@
         <v>86</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="8">
+        <v>31</v>
+      </c>
+      <c r="E54" s="7">
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H54" s="10">
-        <v>1</v>
-      </c>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
+      <c r="H54" s="9">
+        <v>1</v>
+      </c>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
@@ -2483,19 +2488,19 @@
         <v>86</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E55" s="8">
+        <v>32</v>
+      </c>
+      <c r="E55" s="7">
         <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H55" s="10">
-        <v>1</v>
-      </c>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
+      <c r="H55" s="9">
+        <v>1</v>
+      </c>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
@@ -2505,19 +2510,19 @@
         <v>86</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="8">
+        <v>33</v>
+      </c>
+      <c r="E56" s="7">
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H56" s="10">
-        <v>1</v>
-      </c>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
+      <c r="H56" s="9">
+        <v>1</v>
+      </c>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
@@ -2527,19 +2532,19 @@
         <v>86</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="8">
+        <v>34</v>
+      </c>
+      <c r="E57" s="7">
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H57" s="10">
-        <v>1</v>
-      </c>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
+      <c r="H57" s="9">
+        <v>1</v>
+      </c>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
@@ -2549,19 +2554,19 @@
         <v>86</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E58" s="8">
+        <v>35</v>
+      </c>
+      <c r="E58" s="7">
         <v>1</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H58" s="10">
-        <v>1</v>
-      </c>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
+      <c r="H58" s="9">
+        <v>1</v>
+      </c>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
@@ -2571,19 +2576,19 @@
         <v>86</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E59" s="8">
+        <v>36</v>
+      </c>
+      <c r="E59" s="7">
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H59" s="10">
-        <v>1</v>
-      </c>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
+      <c r="H59" s="9">
+        <v>1</v>
+      </c>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
@@ -2593,19 +2598,19 @@
         <v>86</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="8">
+        <v>37</v>
+      </c>
+      <c r="E60" s="7">
         <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H60" s="10">
-        <v>1</v>
-      </c>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
+      <c r="H60" s="9">
+        <v>1</v>
+      </c>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
@@ -2615,61 +2620,69 @@
         <v>86</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E61" s="8">
+        <v>38</v>
+      </c>
+      <c r="E61" s="7">
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H61" s="10">
-        <v>1</v>
-      </c>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
+      <c r="H61" s="9">
+        <v>1</v>
+      </c>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E62" s="8">
-        <v>1</v>
-      </c>
-      <c r="F62" s="8">
+        <v>39</v>
+      </c>
+      <c r="E62" s="7">
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H62" s="8">
-        <v>1</v>
-      </c>
-      <c r="I62" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>153</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="H62" s="9">
+        <v>1</v>
+      </c>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
-        <v>3</v>
-      </c>
       <c r="C63" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="E63" s="7">
+        <v>1</v>
+      </c>
+      <c r="F63" s="7">
+        <v>1</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H63" s="7">
+        <v>1</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2677,56 +2690,56 @@
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>64</v>
       </c>
+      <c r="B65" s="2">
+        <v>1</v>
+      </c>
       <c r="C65" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E65" s="8">
-        <v>1</v>
-      </c>
-      <c r="F65" s="8">
-        <v>1</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H65" s="8">
-        <v>1</v>
-      </c>
-      <c r="I65" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J65" s="8" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
-      <c r="B66" s="2">
-        <v>3</v>
-      </c>
       <c r="C66" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="E66" s="7">
+        <v>1</v>
+      </c>
+      <c r="F66" s="7">
+        <v>1</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H66" s="7">
+        <v>1</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -2734,13 +2747,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -2748,13 +2761,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -2762,13 +2775,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -2776,13 +2789,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -2790,13 +2803,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -2804,13 +2817,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -2818,42 +2831,27 @@
         <v>72</v>
       </c>
       <c r="B73" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>73</v>
       </c>
+      <c r="B74" s="2">
+        <v>1</v>
+      </c>
       <c r="C74" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E74" s="8">
-        <v>1</v>
-      </c>
-      <c r="F74" s="8">
-        <v>1</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H74" s="8">
-        <v>1</v>
-      </c>
-      <c r="I74" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -2864,24 +2862,24 @@
         <v>87</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E75" s="8">
-        <v>1</v>
-      </c>
-      <c r="F75" s="8">
+        <v>100</v>
+      </c>
+      <c r="E75" s="7">
+        <v>1</v>
+      </c>
+      <c r="F75" s="7">
         <v>1</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H75" s="8">
-        <v>1</v>
-      </c>
-      <c r="I75" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J75" s="8" t="s">
+      <c r="H75" s="7">
+        <v>1</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J75" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2893,24 +2891,24 @@
         <v>87</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E76" s="8">
-        <v>1</v>
-      </c>
-      <c r="F76" s="8">
+        <v>101</v>
+      </c>
+      <c r="E76" s="7">
+        <v>1</v>
+      </c>
+      <c r="F76" s="7">
         <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H76" s="8">
-        <v>1</v>
-      </c>
-      <c r="I76" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J76" s="8" t="s">
+      <c r="H76" s="7">
+        <v>1</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J76" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2922,24 +2920,24 @@
         <v>87</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E77" s="8">
-        <v>1</v>
-      </c>
-      <c r="F77" s="8">
+        <v>102</v>
+      </c>
+      <c r="E77" s="7">
+        <v>1</v>
+      </c>
+      <c r="F77" s="7">
         <v>1</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H77" s="8">
-        <v>1</v>
-      </c>
-      <c r="I77" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J77" s="8" t="s">
+      <c r="H77" s="7">
+        <v>1</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J77" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2951,50 +2949,54 @@
         <v>87</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E78" s="8">
-        <v>1</v>
-      </c>
-      <c r="F78" s="8">
+        <v>103</v>
+      </c>
+      <c r="E78" s="7">
+        <v>1</v>
+      </c>
+      <c r="F78" s="7">
         <v>1</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H78" s="8">
-        <v>1</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J78" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="7">
+        <v>1</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>78</v>
       </c>
-      <c r="B79" s="2">
-        <v>4</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>124</v>
+      <c r="C79" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
+        <v>104</v>
+      </c>
+      <c r="E79" s="7">
+        <v>1</v>
+      </c>
+      <c r="F79" s="7">
+        <v>1</v>
+      </c>
       <c r="G79" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="2" t="s">
-        <v>125</v>
+        <v>87</v>
+      </c>
+      <c r="H79" s="7">
+        <v>1</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J79" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3008,21 +3010,21 @@
         <v>124</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
       <c r="G80" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
       <c r="K80" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -3033,16 +3035,21 @@
         <v>124</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
       <c r="G81" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
       <c r="K81" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>81</v>
       </c>
@@ -3053,21 +3060,16 @@
         <v>124</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
+        <v>119</v>
+      </c>
       <c r="G82" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
       <c r="K82" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>82</v>
       </c>
@@ -3078,74 +3080,70 @@
         <v>124</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>121</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
       <c r="G83" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
       <c r="K83" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>83</v>
       </c>
-      <c r="B84" s="2"/>
+      <c r="B84" s="2">
+        <v>4</v>
+      </c>
       <c r="C84" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E84" s="8">
-        <v>1</v>
-      </c>
-      <c r="F84" s="8">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H84" s="8">
-        <v>1</v>
-      </c>
-      <c r="I84" s="8">
-        <v>1</v>
-      </c>
-      <c r="J84" s="8">
-        <v>1</v>
-      </c>
-      <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>84</v>
       </c>
+      <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" s="8">
-        <v>1</v>
-      </c>
-      <c r="F85" s="8">
+        <v>59</v>
+      </c>
+      <c r="E85" s="7">
+        <v>1</v>
+      </c>
+      <c r="F85" s="7">
         <v>1</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H85" s="8">
-        <v>1</v>
-      </c>
-      <c r="I85" s="8">
-        <v>1</v>
-      </c>
-      <c r="J85" s="8">
-        <v>1</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H85" s="7">
+        <v>1</v>
+      </c>
+      <c r="I85" s="7">
+        <v>1</v>
+      </c>
+      <c r="J85" s="7">
+        <v>1</v>
+      </c>
+      <c r="K85" s="2"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
@@ -3155,24 +3153,24 @@
         <v>124</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E86" s="8">
-        <v>1</v>
-      </c>
-      <c r="F86" s="8">
+        <v>6</v>
+      </c>
+      <c r="E86" s="7">
+        <v>1</v>
+      </c>
+      <c r="F86" s="7">
         <v>1</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" s="8">
-        <v>1</v>
-      </c>
-      <c r="I86" s="8">
-        <v>1</v>
-      </c>
-      <c r="J86" s="8">
+        <v>6</v>
+      </c>
+      <c r="H86" s="7">
+        <v>1</v>
+      </c>
+      <c r="I86" s="7">
+        <v>1</v>
+      </c>
+      <c r="J86" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3180,17 +3178,29 @@
       <c r="A87" s="6">
         <v>86</v>
       </c>
-      <c r="B87" s="2">
-        <v>3</v>
-      </c>
       <c r="C87" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>112</v>
+        <v>8</v>
+      </c>
+      <c r="E87" s="7">
+        <v>1</v>
+      </c>
+      <c r="F87" s="7">
+        <v>1</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>106</v>
+        <v>8</v>
+      </c>
+      <c r="H87" s="7">
+        <v>1</v>
+      </c>
+      <c r="I87" s="7">
+        <v>1</v>
+      </c>
+      <c r="J87" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -3198,77 +3208,65 @@
         <v>87</v>
       </c>
       <c r="B88" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
         <v>88</v>
       </c>
-      <c r="B89" s="2"/>
+      <c r="B89" s="2">
+        <v>2</v>
+      </c>
       <c r="C89" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E89" s="8">
-        <v>1</v>
-      </c>
-      <c r="F89" s="8">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H89" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I89" s="8">
-        <v>1</v>
-      </c>
-      <c r="J89" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K89" s="2"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>89</v>
       </c>
+      <c r="B90" s="2"/>
       <c r="C90" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E90" s="8">
-        <v>1</v>
-      </c>
-      <c r="F90" s="8">
+        <v>77</v>
+      </c>
+      <c r="E90" s="7">
+        <v>1</v>
+      </c>
+      <c r="F90" s="7">
         <v>1</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H90" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I90" s="8">
-        <v>1</v>
-      </c>
-      <c r="J90" s="8" t="s">
-        <v>153</v>
-      </c>
+      <c r="H90" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I90" s="7">
+        <v>1</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K90" s="2"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
@@ -3278,24 +3276,24 @@
         <v>124</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E91" s="8">
-        <v>1</v>
-      </c>
-      <c r="F91" s="8">
+        <v>3</v>
+      </c>
+      <c r="E91" s="7">
+        <v>1</v>
+      </c>
+      <c r="F91" s="7">
         <v>1</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H91" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I91" s="8">
-        <v>1</v>
-      </c>
-      <c r="J91" s="8" t="s">
+      <c r="H91" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I91" s="7">
+        <v>1</v>
+      </c>
+      <c r="J91" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3307,24 +3305,24 @@
         <v>124</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E92" s="8">
-        <v>1</v>
-      </c>
-      <c r="F92" s="8">
+        <v>78</v>
+      </c>
+      <c r="E92" s="7">
+        <v>1</v>
+      </c>
+      <c r="F92" s="7">
         <v>1</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H92" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I92" s="8">
-        <v>1</v>
-      </c>
-      <c r="J92" s="8" t="s">
+      <c r="H92" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I92" s="7">
+        <v>1</v>
+      </c>
+      <c r="J92" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3336,24 +3334,24 @@
         <v>124</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E93" s="8">
-        <v>1</v>
-      </c>
-      <c r="F93" s="8">
+        <v>79</v>
+      </c>
+      <c r="E93" s="7">
+        <v>1</v>
+      </c>
+      <c r="F93" s="7">
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H93" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I93" s="8">
-        <v>1</v>
-      </c>
-      <c r="J93" s="8" t="s">
+      <c r="H93" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I93" s="7">
+        <v>1</v>
+      </c>
+      <c r="J93" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3365,24 +3363,24 @@
         <v>124</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="8">
-        <v>1</v>
-      </c>
-      <c r="F94" s="8">
+        <v>109</v>
+      </c>
+      <c r="E94" s="7">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7">
         <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H94" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I94" s="8">
-        <v>1</v>
-      </c>
-      <c r="J94" s="8" t="s">
+      <c r="H94" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I94" s="7">
+        <v>1</v>
+      </c>
+      <c r="J94" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3394,24 +3392,24 @@
         <v>124</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E95" s="8">
-        <v>1</v>
-      </c>
-      <c r="F95" s="8">
+        <v>9</v>
+      </c>
+      <c r="E95" s="7">
+        <v>1</v>
+      </c>
+      <c r="F95" s="7">
         <v>1</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H95" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I95" s="8">
-        <v>1</v>
-      </c>
-      <c r="J95" s="8" t="s">
+      <c r="H95" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I95" s="7">
+        <v>1</v>
+      </c>
+      <c r="J95" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3423,24 +3421,24 @@
         <v>124</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E96" s="8">
-        <v>1</v>
-      </c>
-      <c r="F96" s="8">
+        <v>10</v>
+      </c>
+      <c r="E96" s="7">
+        <v>1</v>
+      </c>
+      <c r="F96" s="7">
         <v>1</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H96" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I96" s="8">
-        <v>1</v>
-      </c>
-      <c r="J96" s="8" t="s">
+      <c r="H96" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I96" s="7">
+        <v>1</v>
+      </c>
+      <c r="J96" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3452,24 +3450,24 @@
         <v>124</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E97" s="8">
-        <v>1</v>
-      </c>
-      <c r="F97" s="8">
+        <v>11</v>
+      </c>
+      <c r="E97" s="7">
+        <v>1</v>
+      </c>
+      <c r="F97" s="7">
         <v>1</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H97" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I97" s="8">
-        <v>1</v>
-      </c>
-      <c r="J97" s="8" t="s">
+      <c r="H97" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I97" s="7">
+        <v>1</v>
+      </c>
+      <c r="J97" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3481,25 +3479,25 @@
         <v>124</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E98" s="8">
-        <v>1</v>
-      </c>
-      <c r="F98" s="8">
+        <v>111</v>
+      </c>
+      <c r="E98" s="7">
+        <v>1</v>
+      </c>
+      <c r="F98" s="7">
         <v>1</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H98" s="8">
-        <v>1</v>
-      </c>
-      <c r="I98" s="8">
-        <v>1</v>
-      </c>
-      <c r="J98" s="8">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="H98" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I98" s="7">
+        <v>1</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -3510,24 +3508,24 @@
         <v>124</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E99" s="8">
-        <v>1</v>
-      </c>
-      <c r="F99" s="8">
+        <v>114</v>
+      </c>
+      <c r="E99" s="7">
+        <v>1</v>
+      </c>
+      <c r="F99" s="7">
         <v>1</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H99" s="8">
-        <v>1</v>
-      </c>
-      <c r="I99" s="8">
-        <v>1</v>
-      </c>
-      <c r="J99" s="8">
+      <c r="H99" s="7">
+        <v>1</v>
+      </c>
+      <c r="I99" s="7">
+        <v>1</v>
+      </c>
+      <c r="J99" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3539,45 +3537,57 @@
         <v>124</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E100" s="8">
-        <v>1</v>
-      </c>
-      <c r="F100" s="8">
+        <v>115</v>
+      </c>
+      <c r="E100" s="7">
+        <v>1</v>
+      </c>
+      <c r="F100" s="7">
         <v>1</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H100" s="8">
-        <v>1</v>
-      </c>
-      <c r="I100" s="8">
-        <v>1</v>
-      </c>
-      <c r="J100" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H100" s="7">
+        <v>1</v>
+      </c>
+      <c r="I100" s="7">
+        <v>1</v>
+      </c>
+      <c r="J100" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>100</v>
       </c>
-      <c r="B101" s="2">
-        <v>1</v>
-      </c>
       <c r="C101" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>66</v>
+        <v>116</v>
+      </c>
+      <c r="E101" s="7">
+        <v>1</v>
+      </c>
+      <c r="F101" s="7">
+        <v>1</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="H101" s="7">
+        <v>1</v>
+      </c>
+      <c r="I101" s="7">
+        <v>1</v>
+      </c>
+      <c r="J101" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>101</v>
       </c>
@@ -3588,33 +3598,34 @@
         <v>124</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>122</v>
+        <v>66</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>102</v>
       </c>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4" t="s">
+      <c r="B103" s="2">
+        <v>4</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F103" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G103" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="4"/>
+      <c r="D103" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
@@ -3625,20 +3636,20 @@
         <v>124</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E104" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F104" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="J104" s="10"/>
       <c r="K104" s="4"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -3650,20 +3661,20 @@
         <v>124</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E105" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F105" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F105" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G105" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
       <c r="K105" s="4"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -3675,20 +3686,20 @@
         <v>124</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F106" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F106" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G106" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="11"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
       <c r="K106" s="4"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -3700,43 +3711,46 @@
         <v>124</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F107" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F107" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="11"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
       <c r="K107" s="4"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>107</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E108" s="8">
-        <v>1</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H108" s="8">
-        <v>1</v>
-      </c>
-      <c r="I108" s="15"/>
-      <c r="J108" s="15"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F108" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="10"/>
+      <c r="K108" s="4"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
@@ -3746,19 +3760,19 @@
         <v>126</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E109" s="8">
+        <v>112</v>
+      </c>
+      <c r="E109" s="7">
         <v>1</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H109" s="8">
-        <v>1</v>
-      </c>
-      <c r="I109" s="15"/>
-      <c r="J109" s="15"/>
+      <c r="H109" s="7">
+        <v>1</v>
+      </c>
+      <c r="I109" s="14"/>
+      <c r="J109" s="14"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
@@ -3768,19 +3782,19 @@
         <v>126</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E110" s="8">
+        <v>139</v>
+      </c>
+      <c r="E110" s="7">
         <v>1</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H110" s="8">
-        <v>1</v>
-      </c>
-      <c r="I110" s="15"/>
-      <c r="J110" s="15"/>
+      <c r="H110" s="7">
+        <v>1</v>
+      </c>
+      <c r="I110" s="14"/>
+      <c r="J110" s="14"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
@@ -3790,19 +3804,19 @@
         <v>126</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E111" s="8">
+        <v>140</v>
+      </c>
+      <c r="E111" s="7">
         <v>1</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H111" s="8">
-        <v>1</v>
-      </c>
-      <c r="I111" s="15"/>
-      <c r="J111" s="15"/>
+      <c r="H111" s="7">
+        <v>1</v>
+      </c>
+      <c r="I111" s="14"/>
+      <c r="J111" s="14"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
@@ -3812,19 +3826,19 @@
         <v>126</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E112" s="8">
+        <v>141</v>
+      </c>
+      <c r="E112" s="7">
         <v>1</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H112" s="8">
-        <v>1</v>
-      </c>
-      <c r="I112" s="15"/>
-      <c r="J112" s="15"/>
+        <v>149</v>
+      </c>
+      <c r="H112" s="7">
+        <v>1</v>
+      </c>
+      <c r="I112" s="14"/>
+      <c r="J112" s="14"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
@@ -3834,19 +3848,19 @@
         <v>126</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E113" s="8">
+        <v>113</v>
+      </c>
+      <c r="E113" s="7">
         <v>1</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H113" s="8">
-        <v>1</v>
-      </c>
-      <c r="I113" s="15"/>
-      <c r="J113" s="15"/>
+      <c r="H113" s="7">
+        <v>1</v>
+      </c>
+      <c r="I113" s="14"/>
+      <c r="J113" s="14"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
@@ -3856,19 +3870,19 @@
         <v>126</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E114" s="8">
+        <v>132</v>
+      </c>
+      <c r="E114" s="7">
         <v>1</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H114" s="8">
-        <v>1</v>
-      </c>
-      <c r="I114" s="15"/>
-      <c r="J114" s="15"/>
+      <c r="H114" s="7">
+        <v>1</v>
+      </c>
+      <c r="I114" s="14"/>
+      <c r="J114" s="14"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
@@ -3878,19 +3892,19 @@
         <v>126</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E115" s="8">
+        <v>133</v>
+      </c>
+      <c r="E115" s="7">
         <v>1</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H115" s="8">
-        <v>1</v>
-      </c>
-      <c r="I115" s="15"/>
-      <c r="J115" s="15"/>
+      <c r="H115" s="7">
+        <v>1</v>
+      </c>
+      <c r="I115" s="14"/>
+      <c r="J115" s="14"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
@@ -3900,26 +3914,19 @@
         <v>126</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E116" s="8">
-        <v>1</v>
-      </c>
-      <c r="F116" s="8">
+        <v>134</v>
+      </c>
+      <c r="E116" s="7">
         <v>1</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="H116" s="8">
-        <v>1</v>
-      </c>
-      <c r="I116" s="8">
-        <v>1</v>
-      </c>
-      <c r="J116" s="8">
-        <v>1</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="H116" s="7">
+        <v>1</v>
+      </c>
+      <c r="I116" s="14"/>
+      <c r="J116" s="14"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
@@ -3929,24 +3936,24 @@
         <v>126</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E117" s="8">
-        <v>1</v>
-      </c>
-      <c r="F117" s="8">
+        <v>122</v>
+      </c>
+      <c r="E117" s="7">
+        <v>1</v>
+      </c>
+      <c r="F117" s="7">
         <v>1</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H117" s="8">
-        <v>1</v>
-      </c>
-      <c r="I117" s="8">
-        <v>1</v>
-      </c>
-      <c r="J117" s="8">
+      <c r="H117" s="7">
+        <v>1</v>
+      </c>
+      <c r="I117" s="7">
+        <v>1</v>
+      </c>
+      <c r="J117" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3958,24 +3965,24 @@
         <v>126</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E118" s="8">
-        <v>1</v>
-      </c>
-      <c r="F118" s="8">
+        <v>135</v>
+      </c>
+      <c r="E118" s="7">
+        <v>1</v>
+      </c>
+      <c r="F118" s="7">
         <v>1</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H118" s="8">
-        <v>1</v>
-      </c>
-      <c r="I118" s="8">
-        <v>1</v>
-      </c>
-      <c r="J118" s="8">
+      <c r="H118" s="7">
+        <v>1</v>
+      </c>
+      <c r="I118" s="7">
+        <v>1</v>
+      </c>
+      <c r="J118" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3987,263 +3994,292 @@
         <v>126</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E119" s="8">
-        <v>1</v>
-      </c>
-      <c r="F119" s="8">
+        <v>136</v>
+      </c>
+      <c r="E119" s="7">
+        <v>1</v>
+      </c>
+      <c r="F119" s="7">
         <v>1</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H119" s="8">
-        <v>1</v>
-      </c>
-      <c r="I119" s="8">
-        <v>1</v>
-      </c>
-      <c r="J119" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="7">
+      <c r="H119" s="7">
+        <v>1</v>
+      </c>
+      <c r="I119" s="7">
+        <v>1</v>
+      </c>
+      <c r="J119" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="6">
         <v>119</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C120" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D120" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F120" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H120" s="11"/>
-      <c r="I120" s="11"/>
-      <c r="J120" s="11"/>
+      <c r="D120" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E120" s="7">
+        <v>1</v>
+      </c>
+      <c r="F120" s="7">
+        <v>1</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H120" s="7">
+        <v>1</v>
+      </c>
+      <c r="I120" s="7">
+        <v>1</v>
+      </c>
+      <c r="J120" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="7">
+      <c r="A121" s="6">
         <v>120</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E121" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F121" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F121" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H121" s="11"/>
-      <c r="I121" s="11"/>
-      <c r="J121" s="11"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+      <c r="J121" s="10"/>
     </row>
     <row r="122" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="7">
+      <c r="A122" s="6">
         <v>121</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E122" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F122" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F122" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H122" s="11"/>
-      <c r="I122" s="11"/>
-      <c r="J122" s="11"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="J122" s="10"/>
     </row>
     <row r="123" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="7">
+      <c r="A123" s="6">
         <v>122</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E123" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F123" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F123" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H123" s="11"/>
-      <c r="I123" s="11"/>
-      <c r="J123" s="11"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="J123" s="10"/>
     </row>
     <row r="124" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="7">
+      <c r="A124" s="6">
         <v>123</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E124" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F124" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F124" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H124" s="11"/>
-      <c r="I124" s="11"/>
-      <c r="J124" s="11"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="J124" s="10"/>
     </row>
     <row r="125" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="7">
+      <c r="A125" s="6">
         <v>124</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E125" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F125" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F125" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H125" s="11"/>
-      <c r="I125" s="11"/>
-      <c r="J125" s="11"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="J125" s="10"/>
     </row>
     <row r="126" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="7">
+      <c r="A126" s="6">
         <v>125</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E126" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F126" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F126" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H126" s="11"/>
-      <c r="I126" s="11"/>
-      <c r="J126" s="11"/>
+      <c r="H126" s="10"/>
+      <c r="I126" s="10"/>
+      <c r="J126" s="10"/>
     </row>
     <row r="127" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="7">
+      <c r="A127" s="6">
         <v>126</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E127" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F127" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F127" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G127" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H127" s="11"/>
-      <c r="I127" s="11"/>
-      <c r="J127" s="11"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10"/>
     </row>
     <row r="128" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="7">
+      <c r="A128" s="6">
         <v>127</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E128" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F128" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E128" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F128" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H128" s="11"/>
-      <c r="I128" s="11"/>
-      <c r="J128" s="11"/>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+      <c r="J128" s="10"/>
     </row>
     <row r="129" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="7">
+      <c r="A129" s="6">
         <v>128</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D129" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E129" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F129" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="J129" s="10"/>
+    </row>
+    <row r="130" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="6">
+        <v>129</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E129" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F129" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G129" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H129" s="11"/>
-      <c r="I129" s="11"/>
-      <c r="J129" s="11"/>
+      <c r="E130" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F130" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+      <c r="J130" s="10"/>
     </row>
   </sheetData>
   <sortState ref="A79:K107">
     <sortCondition ref="G79:G107"/>
   </sortState>
   <dataConsolidate/>
-  <conditionalFormatting sqref="B79:B129 B2:C78">
+  <conditionalFormatting sqref="B80:B130 B2:C79">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
error test cases complete
</commit_message>
<xml_diff>
--- a/Test Cases List.xlsx
+++ b/Test Cases List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="160">
   <si>
     <t>Column</t>
   </si>
@@ -214,12 +214,6 @@
     <t>out of date. also, when is it null vs when is it zero? see uid CYP19A1 vs uid CYP19A1_NC in pop_stats</t>
   </si>
   <si>
-    <t>regtest for now, use mupit to find aas in hotspots on certain genes</t>
-  </si>
-  <si>
-    <t>regtest for now, use genes available in mupit</t>
-  </si>
-  <si>
     <t>transcript</t>
   </si>
   <si>
@@ -484,22 +478,28 @@
     <t>-</t>
   </si>
   <si>
-    <t>when does this show up?</t>
-  </si>
-  <si>
     <t>seqont</t>
   </si>
   <si>
     <t>waiting on bugfix</t>
   </si>
   <si>
-    <t>error_t</t>
-  </si>
-  <si>
-    <t>error_c</t>
-  </si>
-  <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>when does this show up for a noncoding</t>
+  </si>
+  <si>
+    <t>if transcript name doesn't match any conventions</t>
+  </si>
+  <si>
+    <t>if len(aa_change) &lt; 3</t>
+  </si>
+  <si>
+    <t>if AA pos contains non numeric characters</t>
+  </si>
+  <si>
+    <t>fails to write error to db.  pivotal bug made</t>
   </si>
 </sst>
 </file>
@@ -558,18 +558,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -584,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,14 +596,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,9 +923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K2:K7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +933,7 @@
     <col min="1" max="1" width="3.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
@@ -950,37 +947,37 @@
   <sheetData>
     <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="J1" s="10">
         <v>18</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -988,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -997,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -1009,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1017,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -1026,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H3" s="7">
         <v>1</v>
@@ -1038,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1046,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
@@ -1055,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -1067,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1075,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>20</v>
@@ -1084,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
@@ -1096,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1104,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
@@ -1113,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
@@ -1125,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1133,7 +1130,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>23</v>
@@ -1157,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1165,7 +1162,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
@@ -1189,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1197,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>27</v>
@@ -1221,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>54</v>
@@ -1232,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>24</v>
@@ -1250,10 +1247,10 @@
         <v>1</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1261,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>25</v>
@@ -1279,10 +1276,10 @@
         <v>1</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1290,7 +1287,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>7</v>
@@ -1314,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>60</v>
@@ -1325,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -1349,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1357,7 +1354,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -1381,77 +1378,77 @@
         <v>1</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>71</v>
+      <c r="E16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1459,10 +1456,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
@@ -1483,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1491,7 +1488,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>22</v>
@@ -1515,10 +1512,10 @@
         <v>1</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1526,7 +1523,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>40</v>
@@ -1550,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1561,10 +1558,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E20" s="6">
         <v>1</v>
@@ -1585,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1593,10 +1590,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E21" s="6">
         <v>1</v>
@@ -1617,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1625,10 +1622,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" s="6">
         <v>1</v>
@@ -1649,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>63</v>
@@ -1660,7 +1657,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>41</v>
@@ -1684,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>56</v>
@@ -1695,7 +1692,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>47</v>
@@ -1719,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>56</v>
@@ -1730,7 +1727,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>42</v>
@@ -1754,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>56</v>
@@ -1765,7 +1762,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
@@ -1789,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>56</v>
@@ -1800,7 +1797,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>44</v>
@@ -1824,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>56</v>
@@ -1835,7 +1832,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>45</v>
@@ -1859,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>56</v>
@@ -1870,7 +1867,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>46</v>
@@ -1894,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>56</v>
@@ -1905,7 +1902,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>48</v>
@@ -1929,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>56</v>
@@ -1940,7 +1937,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>49</v>
@@ -1964,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>56</v>
@@ -1975,7 +1972,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>14</v>
@@ -1999,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2007,7 +2004,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>28</v>
@@ -2016,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H33" s="7">
         <v>1</v>
@@ -2028,7 +2025,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2036,7 +2033,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>29</v>
@@ -2045,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H34" s="7">
         <v>1</v>
@@ -2057,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2065,7 +2062,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>15</v>
@@ -2077,7 +2074,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H35" s="7">
         <v>1</v>
@@ -2089,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2097,30 +2094,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H36" s="7">
         <v>1</v>
       </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="6" t="s">
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2128,30 +2123,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H37" s="7">
         <v>1</v>
       </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="6" t="s">
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2162,22 +2155,19 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
-      <c r="K38" s="6" t="s">
+      <c r="L38" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2185,16 +2175,16 @@
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E39" s="6">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H39" s="7">
         <v>1</v>
@@ -2206,10 +2196,10 @@
         <v>1</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2217,16 +2207,16 @@
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H40" s="7">
         <v>1</v>
@@ -2238,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2249,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>12</v>
@@ -2261,19 +2251,19 @@
         <v>61</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I41" s="6">
         <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>55</v>
@@ -2287,7 +2277,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>52</v>
@@ -2299,22 +2289,22 @@
         <v>61</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I42" s="6">
         <v>1</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2325,25 +2315,25 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I43" s="6">
         <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2351,10 +2341,10 @@
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E44" s="6">
         <v>1</v>
@@ -2363,19 +2353,19 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I44" s="6">
         <v>1</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2383,7 +2373,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>3</v>
@@ -2395,19 +2385,19 @@
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I45" s="6">
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2415,10 +2405,10 @@
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E46" s="6">
         <v>1</v>
@@ -2427,19 +2417,19 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I46" s="6">
         <v>1</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2447,10 +2437,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E47" s="6">
         <v>1</v>
@@ -2459,19 +2449,19 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I47" s="6">
         <v>1</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2479,7 +2469,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>9</v>
@@ -2491,27 +2481,27 @@
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I48" s="6">
         <v>1</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>10</v>
@@ -2523,27 +2513,27 @@
         <v>1</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I49" s="6">
         <v>1</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>11</v>
@@ -2555,27 +2545,27 @@
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I50" s="6">
         <v>1</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>5</v>
@@ -2587,27 +2577,27 @@
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I51" s="6">
         <v>1</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>13</v>
@@ -2619,27 +2609,27 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I52" s="6">
         <v>1</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>30</v>
@@ -2648,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H53" s="7">
         <v>1</v>
@@ -2660,15 +2650,15 @@
         <v>1</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>31</v>
@@ -2677,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H54" s="7">
         <v>1</v>
@@ -2689,15 +2679,15 @@
         <v>1</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>32</v>
@@ -2706,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H55" s="7">
         <v>1</v>
@@ -2718,15 +2708,15 @@
         <v>1</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>33</v>
@@ -2735,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H56" s="7">
         <v>1</v>
@@ -2747,15 +2737,15 @@
         <v>1</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>34</v>
@@ -2764,7 +2754,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H57" s="7">
         <v>1</v>
@@ -2776,15 +2766,15 @@
         <v>1</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>35</v>
@@ -2793,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H58" s="7">
         <v>1</v>
@@ -2805,15 +2795,15 @@
         <v>1</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>36</v>
@@ -2822,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H59" s="7">
         <v>1</v>
@@ -2834,15 +2824,15 @@
         <v>1</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>37</v>
@@ -2851,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H60" s="7">
         <v>1</v>
@@ -2863,15 +2853,15 @@
         <v>1</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>38</v>
@@ -2880,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H61" s="7">
         <v>1</v>
@@ -2892,15 +2882,15 @@
         <v>1</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>39</v>
@@ -2909,7 +2899,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H62" s="7">
         <v>1</v>
@@ -2921,21 +2911,18 @@
         <v>1</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>62</v>
-      </c>
-      <c r="B63" s="2">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E63" s="6">
         <v>1</v>
@@ -2944,33 +2931,30 @@
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H63" s="6">
+        <v>1</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K63" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>63</v>
-      </c>
-      <c r="B64" s="2">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E64" s="6">
         <v>1</v>
@@ -2979,36 +2963,30 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H64" s="6">
+        <v>1</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K64" s="6">
-        <v>1</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>64</v>
-      </c>
-      <c r="B65" s="2">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E65" s="6">
         <v>1</v>
@@ -3017,84 +2995,124 @@
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H65" s="6">
+        <v>1</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K65" s="6">
-        <v>1</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="L65" s="6"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
-        <v>65</v>
-      </c>
-      <c r="B66" s="2">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="E66" s="6">
+        <v>1</v>
+      </c>
+      <c r="F66" s="6">
+        <v>1</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K66" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H66" s="6">
+        <v>1</v>
+      </c>
+      <c r="I66" s="6">
+        <v>1</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K66" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
-        <v>66</v>
-      </c>
-      <c r="B67" s="2">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="E67" s="6">
+        <v>1</v>
+      </c>
+      <c r="F67" s="6">
+        <v>1</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K67" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H67" s="6">
+        <v>1</v>
+      </c>
+      <c r="I67" s="6">
+        <v>1</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <v>67</v>
-      </c>
-      <c r="B68" s="2">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
+      </c>
+      <c r="E68" s="6">
+        <v>1</v>
+      </c>
+      <c r="F68" s="6">
+        <v>1</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K68" s="11"/>
-      <c r="L68" s="2" t="s">
-        <v>156</v>
+        <v>85</v>
+      </c>
+      <c r="H68" s="6">
+        <v>1</v>
+      </c>
+      <c r="I68" s="6">
+        <v>1</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K68" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>100</v>
@@ -3106,27 +3124,27 @@
         <v>1</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="H69" s="6">
         <v>1</v>
       </c>
-      <c r="I69" s="6" t="s">
-        <v>153</v>
+      <c r="I69" s="6">
+        <v>1</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>101</v>
@@ -3138,30 +3156,30 @@
         <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="H70" s="6">
         <v>1</v>
       </c>
-      <c r="I70" s="6" t="s">
-        <v>153</v>
+      <c r="I70" s="6">
+        <v>1</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E71" s="6">
         <v>1</v>
@@ -3170,30 +3188,31 @@
         <v>1</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="H71" s="6">
         <v>1</v>
       </c>
-      <c r="I71" s="6" t="s">
-        <v>153</v>
+      <c r="I71" s="6">
+        <v>1</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>153</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="L71" s="15"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E72" s="6">
         <v>1</v>
@@ -3202,59 +3221,56 @@
         <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="H72" s="6">
         <v>1</v>
       </c>
-      <c r="I72" s="6" t="s">
-        <v>153</v>
+      <c r="I72" s="6">
+        <v>1</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K72" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E73" s="6">
-        <v>1</v>
-      </c>
-      <c r="F73" s="6">
-        <v>1</v>
-      </c>
       <c r="G73" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H73" s="6">
-        <v>1</v>
-      </c>
-      <c r="I73" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I73" s="6">
+        <v>1</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+      <c r="L73" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>88</v>
@@ -3266,28 +3282,30 @@
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H74" s="6">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K74" s="11"/>
+        <v>151</v>
+      </c>
+      <c r="K74" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E75" s="6">
         <v>1</v>
@@ -3296,99 +3314,138 @@
         <v>1</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H75" s="6">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K75" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+      <c r="K75" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
-        <v>75</v>
-      </c>
-      <c r="B76" s="2">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="E76" s="6">
+        <v>1</v>
+      </c>
+      <c r="F76" s="6">
+        <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K76" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K76" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
-        <v>76</v>
-      </c>
-      <c r="B77" s="2">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K77" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K77" s="6">
+        <v>1</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
-        <v>77</v>
-      </c>
-      <c r="B78" s="2">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K78" s="6">
+        <v>1</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
-        <v>78</v>
-      </c>
-      <c r="B79" s="2">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K79" s="6" t="s">
-        <v>153</v>
+        <v>85</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K79" s="6">
+        <v>1</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3399,10 +3456,10 @@
         <v>4</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -3413,10 +3470,10 @@
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3427,10 +3484,10 @@
         <v>4</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
@@ -3441,10 +3498,10 @@
       <c r="I81" s="6"/>
       <c r="J81" s="6"/>
       <c r="K81" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -3455,19 +3512,19 @@
         <v>4</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>61</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3478,10 +3535,10 @@
         <v>4</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
@@ -3492,10 +3549,10 @@
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -3506,19 +3563,19 @@
         <v>4</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>61</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3527,7 +3584,7 @@
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>59</v>
@@ -3551,7 +3608,7 @@
         <v>1</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L85" s="2"/>
     </row>
@@ -3560,7 +3617,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>6</v>
@@ -3584,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -3592,7 +3649,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>8</v>
@@ -3616,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -3627,16 +3684,16 @@
         <v>2</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -3647,16 +3704,16 @@
         <v>2</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3665,10 +3722,10 @@
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E90" s="6">
         <v>1</v>
@@ -3677,19 +3734,19 @@
         <v>1</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I90" s="6">
         <v>1</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L90" s="2"/>
     </row>
@@ -3698,7 +3755,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>3</v>
@@ -3710,19 +3767,19 @@
         <v>1</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I91" s="6">
         <v>1</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -3730,10 +3787,10 @@
         <v>91</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E92" s="6">
         <v>1</v>
@@ -3742,19 +3799,19 @@
         <v>1</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I92" s="6">
         <v>1</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -3762,10 +3819,10 @@
         <v>92</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E93" s="6">
         <v>1</v>
@@ -3774,19 +3831,19 @@
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I93" s="6">
         <v>1</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -3794,10 +3851,10 @@
         <v>93</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E94" s="6">
         <v>1</v>
@@ -3806,19 +3863,19 @@
         <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I94" s="6">
         <v>1</v>
       </c>
       <c r="J94" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K94" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -3826,7 +3883,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>9</v>
@@ -3838,19 +3895,19 @@
         <v>1</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I95" s="6">
         <v>1</v>
       </c>
       <c r="J95" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K95" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -3858,7 +3915,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>10</v>
@@ -3870,19 +3927,19 @@
         <v>1</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I96" s="6">
         <v>1</v>
       </c>
       <c r="J96" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K96" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -3890,7 +3947,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>11</v>
@@ -3902,19 +3959,19 @@
         <v>1</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I97" s="6">
         <v>1</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -3922,10 +3979,10 @@
         <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E98" s="6">
         <v>1</v>
@@ -3934,19 +3991,19 @@
         <v>1</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I98" s="6">
         <v>1</v>
       </c>
       <c r="J98" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K98" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -3954,10 +4011,10 @@
         <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E99" s="6">
         <v>1</v>
@@ -3978,7 +4035,7 @@
         <v>1</v>
       </c>
       <c r="K99" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -3986,10 +4043,10 @@
         <v>99</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E100" s="6">
         <v>1</v>
@@ -4010,7 +4067,7 @@
         <v>1</v>
       </c>
       <c r="K100" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -4018,10 +4075,10 @@
         <v>100</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E101" s="6">
         <v>1</v>
@@ -4042,7 +4099,7 @@
         <v>1</v>
       </c>
       <c r="K101" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4053,10 +4110,10 @@
         <v>4</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>61</v>
@@ -4065,13 +4122,13 @@
         <v>61</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K102" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -4082,173 +4139,173 @@
         <v>4</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K103" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>103</v>
       </c>
-      <c r="C104" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D104" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E104" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F104" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G104" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I104" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J104" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K104" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E104" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H104" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I104" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J104" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K104" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>104</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E105" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F105" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G105" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H105" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I105" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J105" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K105" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E105" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G105" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H105" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I105" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J105" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K105" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>105</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D106" s="12" t="s">
+      <c r="C106" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D106" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E106" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F106" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H106" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I106" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J106" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K106" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E106" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H106" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I106" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J106" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K106" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>106</v>
       </c>
-      <c r="C107" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D107" s="12" t="s">
+      <c r="C107" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D107" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E107" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F107" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G107" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I107" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J107" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K107" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E107" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H107" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I107" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J107" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K107" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>107</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F108" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G108" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H108" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I108" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J108" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K108" s="13" t="s">
-        <v>153</v>
+      <c r="C108" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G108" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H108" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I108" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J108" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K108" s="12" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -4256,16 +4313,16 @@
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E109" s="6">
         <v>1</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H109" s="7">
         <v>1</v>
@@ -4277,7 +4334,7 @@
         <v>1</v>
       </c>
       <c r="K109" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -4285,16 +4342,16 @@
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E110" s="6">
         <v>1</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H110" s="7">
         <v>1</v>
@@ -4306,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -4314,16 +4371,16 @@
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E111" s="6">
         <v>1</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H111" s="7">
         <v>1</v>
@@ -4335,7 +4392,7 @@
         <v>1</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
@@ -4343,16 +4400,16 @@
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E112" s="6">
         <v>1</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H112" s="7">
         <v>1</v>
@@ -4364,7 +4421,7 @@
         <v>1</v>
       </c>
       <c r="K112" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -4372,16 +4429,16 @@
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E113" s="6">
         <v>1</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H113" s="7">
         <v>1</v>
@@ -4393,7 +4450,7 @@
         <v>1</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
@@ -4401,16 +4458,16 @@
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E114" s="6">
         <v>1</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H114" s="7">
         <v>1</v>
@@ -4422,7 +4479,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
@@ -4430,16 +4487,16 @@
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E115" s="6">
         <v>1</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H115" s="7">
         <v>1</v>
@@ -4451,7 +4508,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -4459,16 +4516,16 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E116" s="6">
         <v>1</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H116" s="7">
         <v>1</v>
@@ -4480,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="K116" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -4488,10 +4545,10 @@
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E117" s="6">
         <v>1</v>
@@ -4500,7 +4557,7 @@
         <v>1</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H117" s="6">
         <v>1</v>
@@ -4512,7 +4569,7 @@
         <v>1</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -4520,10 +4577,10 @@
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E118" s="6">
         <v>1</v>
@@ -4532,7 +4589,7 @@
         <v>1</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H118" s="6">
         <v>1</v>
@@ -4544,7 +4601,7 @@
         <v>1</v>
       </c>
       <c r="K118" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -4552,10 +4609,10 @@
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E119" s="6">
         <v>1</v>
@@ -4564,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H119" s="6">
         <v>1</v>
@@ -4576,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="K119" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -4584,10 +4641,10 @@
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E120" s="6">
         <v>1</v>
@@ -4596,7 +4653,7 @@
         <v>1</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H120" s="6">
         <v>1</v>
@@ -4608,327 +4665,327 @@
         <v>1</v>
       </c>
       <c r="K120" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>120</v>
       </c>
-      <c r="C121" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D121" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E121" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F121" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G121" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H121" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I121" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J121" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K121" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C121" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F121" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H121" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I121" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J121" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K121" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>121</v>
       </c>
-      <c r="C122" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C122" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D122" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E122" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F122" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G122" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H122" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I122" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J122" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K122" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E122" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F122" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H122" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I122" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J122" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K122" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>122</v>
       </c>
-      <c r="C123" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D123" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E123" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F123" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G123" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H123" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I123" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J123" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K123" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C123" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F123" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H123" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I123" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J123" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K123" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>123</v>
       </c>
-      <c r="C124" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D124" s="12" t="s">
+      <c r="C124" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D124" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E124" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F124" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G124" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H124" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I124" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J124" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K124" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E124" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F124" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G124" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H124" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I124" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J124" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K124" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>124</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E125" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F125" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G125" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H125" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I125" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J125" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K125" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C125" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E125" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F125" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H125" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I125" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J125" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K125" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>125</v>
       </c>
-      <c r="C126" s="12" t="s">
+      <c r="C126" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D126" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D126" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E126" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F126" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G126" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H126" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I126" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J126" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K126" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E126" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F126" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G126" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H126" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I126" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J126" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K126" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>126</v>
       </c>
-      <c r="C127" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D127" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E127" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F127" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G127" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H127" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I127" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J127" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K127" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E127" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F127" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H127" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I127" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J127" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K127" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>127</v>
       </c>
-      <c r="C128" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D128" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E128" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F128" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G128" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H128" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I128" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J128" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K128" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C128" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E128" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F128" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H128" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I128" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J128" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K128" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>128</v>
       </c>
-      <c r="C129" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E129" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F129" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G129" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H129" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I129" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J129" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K129" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C129" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E129" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F129" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G129" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H129" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I129" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J129" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K129" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>129</v>
       </c>
-      <c r="C130" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D130" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E130" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F130" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G130" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H130" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I130" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="J130" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="K130" s="13" t="s">
-        <v>153</v>
+      <c r="C130" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E130" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F130" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G130" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H130" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I130" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J130" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K130" s="12" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>